<commit_message>
updated manufacturing files for esp-wiwi
</commit_message>
<xml_diff>
--- a/Incubation/Hardware/ESP-WiWi/Project Outputs for ESP-WiWi/Manufacturing Outputs/BOM/Bill of Materials-ESP-WiWi.xlsx
+++ b/Incubation/Hardware/ESP-WiWi/Project Outputs for ESP-WiWi/Manufacturing Outputs/BOM/Bill of Materials-ESP-WiWi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\My Drive\Meta\TAP\Workspace\esp_wiwi_board\Altium\ESP-WiWi\Project Outputs for ESP-WiWi\Manufacturing Outputs\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DCF1C9B-E2AE-44DF-9947-DD2C88F53A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80FC1723-4508-4483-883C-B383C0173843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3308" yWindow="3308" windowWidth="19440" windowHeight="11872" xr2:uid="{740782A3-B166-4FD6-B4ED-B713A2286311}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="19440" windowHeight="11857" xr2:uid="{05174670-3FBF-4408-B099-E7943E92CDFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-ESP-WiWi" sheetId="1" r:id="rId1"/>
@@ -1321,7 +1321,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A988C5E6-447F-44F1-9758-4806442AC097}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0E95F0-6261-4B53-8D9B-5F1F5571FB89}">
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>